<commit_message>
bot fetch tea File
</commit_message>
<xml_diff>
--- a/tencentdoc/tea.xlsx
+++ b/tencentdoc/tea.xlsx
@@ -490,7 +490,7 @@
           <t>https://codeforces.com/problemset/problem/1610/E
 输入 t(≤1e4) 表示 t 组数据。所有数据的 n 之和 ≤2e5。
 每组数据输入 n(2≤n≤2e5) 和长为 n 的有序数组 a(1≤a[i]≤1e9)，有重复元素。
-你需要从 a 中删除一些元素，对于 a 的任意非空子序列 b，都必须满足：
+你需要从 a 中删除一些元素，使得对于 a 的任意非空子序列 b，都必须满足：
 设 avg 为 b 的平均值（可以是小数），b 中比 avg 小的数的个数必须 &gt;= b 中比 avg 大的数的个数。
 例如 [1,4,4,5,6] 的平均值为 4，有 1 个数比 4 小，有 2 个数比 4 大，这是不满足要求的。
 而 [4,4,5,6] 是满足要求的。
@@ -527,10 +527,11 @@
 设这三个数分别为 x，y，z，那么 y &lt;= avg = (x+y+z)/3，变形得 z &gt;= 2y-x = 2(y-x)+x
 提示 2：在长为 3 的子序列的基础上，增加一个数，这个数需要满足什么性质？
 设增加的数为 u，那么 x，z，u 必须是满足要求的，即 u &gt;= 2z-x &gt;= 2(2y-x)-x = 4y-3x = 4(y-x)+x
-依此类推，增加的数必须 &gt;= 2^k(y-x)+x，这是指数增长的，所以子序列 b 的长度不会超过 log(max(a))。
+依此类推，增加的数必须 &gt;= 2^k*(y-x)+x，这是指数增长的，所以子序列 b 的长度不会超过 log(max(a))。
 这样就可以暴力了，为了让去掉的数尽量少，那么保留的数要尽量多。
-1. y-x 尽量小，那么枚举所有 a[i] 和 a[i+1] 作为 x 和 y。
-2. 从 x,y 开始构建子序列 b，二分找下一个数。</t>
+1. y-x 尽量小（但不能为 0），那么枚举所有 a[i] != a[i+1] 作为 x 和 y。
+2. 从 x,y 开始构建子序列 b，二分找下一个数。
+注意重复元素，所有重复的 x 都可以保留。</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>

</xml_diff>